<commit_message>
User Stories 4 and 6 for Sprint 2
</commit_message>
<xml_diff>
--- a/Team2Report.xlsx
+++ b/Team2Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nsouz\OneDrive\Documents\STEVENS\CS 555 - Agile Methods\Stevens-CS555-Team2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8E53D4-C10A-49AF-963E-B1558EAF1338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29129355-E0B6-4B1A-8ECB-EAEAD58B8690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="187">
   <si>
     <t>Initials</t>
   </si>
@@ -600,6 +600,9 @@
   </si>
   <si>
     <t>Jrossi3</t>
+  </si>
+  <si>
+    <t>NS</t>
   </si>
 </sst>
 </file>
@@ -3122,7 +3125,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:C13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3237,7 +3240,9 @@
       <c r="D5" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="E5" s="18"/>
+      <c r="E5" s="18" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17">
@@ -3250,7 +3255,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>183</v>
@@ -3267,7 +3272,10 @@
         <v>54</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>166</v>
+        <v>186</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3343,7 +3351,7 @@
         <v>74</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3357,7 +3365,7 @@
         <v>77</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -12801,7 +12809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -16967,8 +16975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17015,16 +17023,25 @@
         <v>50</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E2">
         <v>25</v>
       </c>
       <c r="F2">
         <v>120</v>
+      </c>
+      <c r="G2">
+        <v>25</v>
+      </c>
+      <c r="H2">
+        <v>60</v>
+      </c>
+      <c r="I2" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -17035,16 +17052,25 @@
         <v>54</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E3">
         <v>25</v>
       </c>
       <c r="F3">
         <v>120</v>
+      </c>
+      <c r="G3">
+        <v>25</v>
+      </c>
+      <c r="H3">
+        <v>60</v>
+      </c>
+      <c r="I3" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -17095,7 +17121,7 @@
         <v>74</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>176</v>
@@ -17115,7 +17141,7 @@
         <v>77</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>176</v>
@@ -20383,7 +20409,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:B11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Sprint 2 submission & Team report updates
</commit_message>
<xml_diff>
--- a/Team2Report.xlsx
+++ b/Team2Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nsouz\OneDrive\Documents\STEVENS\CS 555 - Agile Methods\Stevens-CS555-Team2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29129355-E0B6-4B1A-8ECB-EAEAD58B8690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F810B3F-CA01-4404-AF1F-ED038F275BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="191">
   <si>
     <t>Initials</t>
   </si>
@@ -572,9 +572,6 @@
     <t>https://github.com/nathsouza/Stevens-CS555-Team2</t>
   </si>
   <si>
-    <t>pending</t>
-  </si>
-  <si>
     <t>slee51@stevens.edu</t>
   </si>
   <si>
@@ -603,6 +600,21 @@
   </si>
   <si>
     <t>NS</t>
+  </si>
+  <si>
+    <t>-Team collaboration</t>
+  </si>
+  <si>
+    <t>-Time management</t>
+  </si>
+  <si>
+    <t>-Work proactively</t>
+  </si>
+  <si>
+    <t>-Making things too perfect</t>
+  </si>
+  <si>
+    <t>PENDING</t>
   </si>
 </sst>
 </file>
@@ -2069,7 +2081,7 @@
         <v>165</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>174</v>
@@ -2087,7 +2099,7 @@
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3190,7 +3202,7 @@
         <v>163</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3207,7 +3219,7 @@
         <v>163</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3224,7 +3236,7 @@
         <v>169</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3241,7 +3253,7 @@
         <v>169</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3258,7 +3270,7 @@
         <v>169</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3272,10 +3284,10 @@
         <v>54</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3292,7 +3304,7 @@
         <v>166</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3337,7 +3349,7 @@
         <v>163</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -12810,7 +12822,7 @@
   <dimension ref="A1:I995"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B13" sqref="B12:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12867,7 +12879,7 @@
         <v>163</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E2">
         <v>25</v>
@@ -12882,7 +12894,7 @@
         <v>300</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -12896,7 +12908,7 @@
         <v>163</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E3">
         <v>25</v>
@@ -12911,7 +12923,7 @@
         <v>300</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -12925,7 +12937,7 @@
         <v>169</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E4">
         <v>25</v>
@@ -12940,7 +12952,7 @@
         <v>300</v>
       </c>
       <c r="I4" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -12954,7 +12966,7 @@
         <v>169</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E5">
         <v>25</v>
@@ -12969,7 +12981,7 @@
         <v>300</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -12983,7 +12995,7 @@
         <v>166</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E6">
         <v>25</v>
@@ -12998,7 +13010,7 @@
         <v>300</v>
       </c>
       <c r="I6" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -13012,7 +13024,7 @@
         <v>166</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E7">
         <v>25</v>
@@ -13027,7 +13039,7 @@
         <v>300</v>
       </c>
       <c r="I7" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -13052,13 +13064,13 @@
     </row>
     <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I13" s="4"/>
     </row>
@@ -13081,7 +13093,7 @@
     </row>
     <row r="18" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I18" s="4"/>
     </row>
@@ -13091,7 +13103,7 @@
     </row>
     <row r="20" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I20" s="4"/>
     </row>
@@ -16975,8 +16987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17026,7 +17038,7 @@
         <v>169</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E2">
         <v>25</v>
@@ -17041,7 +17053,7 @@
         <v>60</v>
       </c>
       <c r="I2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -17055,7 +17067,7 @@
         <v>169</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E3">
         <v>25</v>
@@ -17070,7 +17082,7 @@
         <v>60</v>
       </c>
       <c r="I3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -17084,13 +17096,22 @@
         <v>163</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E4">
         <v>25</v>
       </c>
       <c r="F4">
         <v>120</v>
+      </c>
+      <c r="G4">
+        <v>25</v>
+      </c>
+      <c r="H4">
+        <v>100</v>
+      </c>
+      <c r="I4" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -17104,13 +17125,22 @@
         <v>163</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E5">
         <v>25</v>
       </c>
       <c r="F5">
         <v>120</v>
+      </c>
+      <c r="G5">
+        <v>25</v>
+      </c>
+      <c r="H5">
+        <v>100</v>
+      </c>
+      <c r="I5" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -17124,13 +17154,22 @@
         <v>166</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E6">
         <v>25</v>
       </c>
       <c r="F6">
         <v>120</v>
+      </c>
+      <c r="G6">
+        <v>25</v>
+      </c>
+      <c r="H6">
+        <v>100</v>
+      </c>
+      <c r="I6" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -17144,13 +17183,22 @@
         <v>166</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E7">
         <v>25</v>
       </c>
       <c r="F7">
         <v>120</v>
+      </c>
+      <c r="G7">
+        <v>25</v>
+      </c>
+      <c r="H7">
+        <v>100</v>
+      </c>
+      <c r="I7" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17168,13 +17216,19 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="3"/>
+      <c r="B13" s="3" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="3"/>
+      <c r="B14" s="3" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17186,7 +17240,9 @@
       </c>
     </row>
     <row r="18" spans="2:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="19" spans="2:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
@@ -18191,7 +18247,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C7"/>
+      <selection activeCell="F2" sqref="F2:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -18240,6 +18296,15 @@
       <c r="C2" s="16" t="s">
         <v>163</v>
       </c>
+      <c r="D2" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E2">
+        <v>15</v>
+      </c>
+      <c r="F2">
+        <v>120</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -18251,6 +18316,15 @@
       <c r="C3" s="16" t="s">
         <v>163</v>
       </c>
+      <c r="D3" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E3">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>120</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -18262,6 +18336,15 @@
       <c r="C4" s="16" t="s">
         <v>166</v>
       </c>
+      <c r="D4" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>120</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -18273,6 +18356,15 @@
       <c r="C5" s="16" t="s">
         <v>166</v>
       </c>
+      <c r="D5" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E5">
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <v>120</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -18284,6 +18376,15 @@
       <c r="C6" s="16" t="s">
         <v>169</v>
       </c>
+      <c r="D6" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6">
+        <v>15</v>
+      </c>
+      <c r="F6">
+        <v>120</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -18294,6 +18395,15 @@
       </c>
       <c r="C7" s="16" t="s">
         <v>169</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -20408,8 +20518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>